<commit_message>
Completed rought draft of paper
</commit_message>
<xml_diff>
--- a/Analysis/Paper/Tables.xlsx
+++ b/Analysis/Paper/Tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ta0jrg1\Documents\Projects\Obesity_Redo\Analysis\Paper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4D7DF06-C0E3-4ED3-911C-9336288E476C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8EA9E5A-B318-4F9F-9804-1CFF775C1BAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" firstSheet="9" activeTab="17" xr2:uid="{2117FDC6-2EA3-4270-B58E-054E1375CB25}"/>
   </bookViews>
@@ -8480,8 +8480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{706BF295-AB2E-413A-A9E0-35598F6A239C}">
   <dimension ref="A2:F65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:F65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22035,8 +22035,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63D30258-0279-42C9-AFDD-19DB817A80C5}">
   <dimension ref="A2:F71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D65" sqref="D65"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:F71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>